<commit_message>
cambios en planilla de requerimientos y matriz control de cambio.
</commit_message>
<xml_diff>
--- a/Fase 2/Documentacion/DOCUMENTACION PROYECTO/MATRIZ CONTROL DE CAMBIO.xlsx
+++ b/Fase 2/Documentacion/DOCUMENTACION PROYECTO/MATRIZ CONTROL DE CAMBIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manua\Desktop\pcas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\ProyectoCaps\Fase 2\Documentacion\DOCUMENTACION PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEAEE95-E983-4AEF-AFD7-0D029A32FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31C35C7-ED86-470E-A6AD-735956CE32B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -147,6 +147,31 @@
   </si>
   <si>
     <t>Sin cambios en el proyecto</t>
+  </si>
+  <si>
+    <t>Ignacio Alfaro</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Urgente</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Se realizado la subida del proyecto mediante la aplicacion de render para subirlo a la nube, 
+pero hubo inconvenientes de compatibilidades, asi que se opto por utilizar Clever Cloud</t>
+  </si>
+  <si>
+    <t>Fase 2 del proyecto</t>
+  </si>
+  <si>
+    <t>Aceptado</t>
+  </si>
+  <si>
+    <t>CU001</t>
   </si>
 </sst>
 </file>
@@ -250,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -274,6 +299,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,27 +620,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="82.7109375" customWidth="1"/>
+    <col min="8" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -627,7 +655,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -665,7 +693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -703,23 +731,45 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>45586</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -735,7 +785,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -751,7 +801,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -767,7 +817,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -783,7 +833,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -799,87 +849,87 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>